<commit_message>
demo model and IRI model
- demo model and IRI model
- create publishable tables
</commit_message>
<xml_diff>
--- a/UG_data_analysis/outputs/demographicsgroup4.xlsx
+++ b/UG_data_analysis/outputs/demographicsgroup4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/LAB/Suicide_UG/UG_data_analysis/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B38F20C-DC50-1E4F-87E0-F08A047D36BD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F8DB55-B914-3745-AF66-A6DA10FA0463}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="580" windowWidth="20220" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15640" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="demographicsgroup4" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="100">
   <si>
     <t xml:space="preserve"> N </t>
   </si>
@@ -239,9 +239,6 @@
     <t>Control &lt; Attempter, Ideator</t>
   </si>
   <si>
-    <t>Variables</t>
-  </si>
-  <si>
     <t>% Male</t>
   </si>
   <si>
@@ -315,6 +312,15 @@
   </si>
   <si>
     <t xml:space="preserve">   Affective Empathy</t>
+  </si>
+  <si>
+    <t>BLS</t>
+  </si>
+  <si>
+    <t>3.9 (2.2)</t>
+  </si>
+  <si>
+    <t>Predictors</t>
   </si>
 </sst>
 </file>
@@ -864,7 +870,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -917,6 +923,9 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -980,29 +989,27 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>107950</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>10795</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{561C62E4-F944-7D4F-A008-BFA5A0A3E32A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30A77EE7-F5B8-8446-9024-AE7F410D3B64}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
+        <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
@@ -1012,8 +1019,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="825500" y="3454400"/>
-          <a:ext cx="13804900" cy="5588000"/>
+          <a:off x="2133600" y="7924800"/>
+          <a:ext cx="7054850" cy="2855595"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1322,10 +1329,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:J27"/>
+  <dimension ref="A2:J28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1388,8 +1395,8 @@
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="19">
-      <c r="A5" s="9" t="s">
-        <v>72</v>
+      <c r="A5" s="23" t="s">
+        <v>99</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>66</v>
@@ -1439,7 +1446,7 @@
     </row>
     <row r="7" spans="1:10" ht="19">
       <c r="A7" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" s="11">
         <v>0.51</v>
@@ -1463,7 +1470,7 @@
     </row>
     <row r="8" spans="1:10" ht="19">
       <c r="A8" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" s="12">
         <v>0.83699999999999997</v>
@@ -1513,19 +1520,19 @@
     </row>
     <row r="10" spans="1:10" ht="19">
       <c r="A10" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="E10" s="8" t="s">
         <v>77</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>78</v>
       </c>
       <c r="F10" s="8">
         <v>149</v>
@@ -1539,28 +1546,28 @@
     </row>
     <row r="11" spans="1:10" ht="19">
       <c r="A11" s="6" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>19</v>
+        <v>98</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="F11" s="8">
-        <v>149</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>8</v>
+        <v>49</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="19">
@@ -1568,305 +1575,329 @@
         <v>81</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="F12" s="8">
-        <v>114</v>
+        <v>149</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="J12" s="19" t="s">
-        <v>84</v>
+      <c r="H12" s="13" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="19">
       <c r="A13" s="6" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="F13" s="8">
-        <v>149</v>
-      </c>
-      <c r="G13" s="10">
-        <v>0.16900000000000001</v>
-      </c>
-      <c r="H13" s="13"/>
+        <v>114</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="J13" s="19"/>
     </row>
     <row r="14" spans="1:10" ht="19">
       <c r="A14" s="6" t="s">
-        <v>80</v>
+        <v>14</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="F14" s="8">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="G14" s="10">
-        <v>1.2E-2</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>68</v>
-      </c>
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:10" ht="19">
       <c r="A15" s="6" t="s">
         <v>79</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F15" s="8">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G15" s="10">
-        <v>7.0000000000000001E-3</v>
+        <v>1.2E-2</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="19">
       <c r="A16" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="13"/>
+        <v>78</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="8">
+        <v>144</v>
+      </c>
+      <c r="G16" s="10">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="19">
-      <c r="A17" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="F17" s="22">
-        <v>143</v>
-      </c>
-      <c r="G17" s="22">
-        <v>0.499</v>
-      </c>
+      <c r="A17" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="10"/>
       <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:8" ht="19">
       <c r="A18" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F18" s="22">
         <v>143</v>
       </c>
       <c r="G18" s="22">
+        <v>0.499</v>
+      </c>
+      <c r="H18" s="13"/>
+    </row>
+    <row r="19" spans="1:8" ht="19">
+      <c r="A19" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="22">
+        <v>143</v>
+      </c>
+      <c r="G19" s="22">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="H18" s="21" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="19">
-      <c r="A19" s="6" t="s">
+      <c r="H19" s="21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="19">
+      <c r="A20" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="14"/>
-    </row>
-    <row r="20" spans="1:8" ht="19">
-      <c r="A20" s="14" t="s">
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="14"/>
+    </row>
+    <row r="21" spans="1:8" ht="19">
+      <c r="A21" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B21" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C21" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D21" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E21" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="F20" s="8">
-        <v>142</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="19">
-      <c r="A21" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="F21" s="8">
         <v>142</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="19">
       <c r="A22" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F22" s="8">
         <v>142</v>
       </c>
-      <c r="G22" s="8">
-        <v>1E-3</v>
+      <c r="G22" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="H22" s="13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="20" thickBot="1">
-      <c r="A23" s="15" t="s">
+    <row r="23" spans="1:8" ht="19">
+      <c r="A23" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="8">
+        <v>142</v>
+      </c>
+      <c r="G23" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="20" thickBot="1">
+      <c r="A24" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B24" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C24" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D24" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E24" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F23" s="16">
+      <c r="F24" s="16">
         <v>142</v>
       </c>
-      <c r="G23" s="16" t="s">
+      <c r="G24" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="17" t="s">
+      <c r="H24" s="17" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="20" thickTop="1">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+    <row r="25" spans="1:8" ht="20" thickTop="1">
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
     </row>
     <row r="27" spans="1:8">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1878,8 +1909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>